<commit_message>
update week 7 v2
</commit_message>
<xml_diff>
--- a/2025-biochem_molbio_score.xlsx
+++ b/2025-biochem_molbio_score.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="471">
   <si>
     <t>ID</t>
   </si>
@@ -8283,10 +8283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1383"/>
+  <dimension ref="A1:E1615"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A901" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G918" sqref="G918"/>
+    <sheetView tabSelected="1" topLeftCell="A1610" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1158" sqref="D1158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -29650,6 +29650,3242 @@
       </c>
       <c r="E1383">
         <v>6</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1384" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1384">
+        <v>100</v>
+      </c>
+      <c r="D1384">
+        <v>100</v>
+      </c>
+      <c r="E1384">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1385" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1385">
+        <v>70</v>
+      </c>
+      <c r="D1385">
+        <v>40</v>
+      </c>
+      <c r="E1385">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1386">
+        <v>80</v>
+      </c>
+      <c r="E1386">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1387">
+        <v>40</v>
+      </c>
+      <c r="D1387">
+        <v>60</v>
+      </c>
+      <c r="E1387">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1388" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1388">
+        <v>90</v>
+      </c>
+      <c r="D1388">
+        <v>80</v>
+      </c>
+      <c r="E1388">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1389" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1389">
+        <v>50</v>
+      </c>
+      <c r="E1389">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1390" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1390">
+        <v>90</v>
+      </c>
+      <c r="E1390">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1391" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1391">
+        <v>100</v>
+      </c>
+      <c r="D1391">
+        <v>100</v>
+      </c>
+      <c r="E1391">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1392" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1392">
+        <v>100</v>
+      </c>
+      <c r="D1392">
+        <v>100</v>
+      </c>
+      <c r="E1392">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1393">
+        <v>90</v>
+      </c>
+      <c r="D1393">
+        <v>80</v>
+      </c>
+      <c r="E1393">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1394" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1394">
+        <v>100</v>
+      </c>
+      <c r="D1394">
+        <v>80</v>
+      </c>
+      <c r="E1394">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1395" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1395">
+        <v>100</v>
+      </c>
+      <c r="D1395">
+        <v>100</v>
+      </c>
+      <c r="E1395">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1396" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1396">
+        <v>30</v>
+      </c>
+      <c r="D1396">
+        <v>60</v>
+      </c>
+      <c r="E1396">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1397" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1397">
+        <v>100</v>
+      </c>
+      <c r="D1397">
+        <v>100</v>
+      </c>
+      <c r="E1397">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1398" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1398">
+        <v>100</v>
+      </c>
+      <c r="D1398">
+        <v>60</v>
+      </c>
+      <c r="E1398">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1399" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1399">
+        <v>90</v>
+      </c>
+      <c r="D1399">
+        <v>60</v>
+      </c>
+      <c r="E1399">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1400" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1400">
+        <v>80</v>
+      </c>
+      <c r="D1400">
+        <v>60</v>
+      </c>
+      <c r="E1400">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1401" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1401">
+        <v>100</v>
+      </c>
+      <c r="D1401">
+        <v>80</v>
+      </c>
+      <c r="E1401">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1402">
+        <v>90</v>
+      </c>
+      <c r="D1402">
+        <v>60</v>
+      </c>
+      <c r="E1402">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1403">
+        <v>70</v>
+      </c>
+      <c r="D1403">
+        <v>60</v>
+      </c>
+      <c r="E1403">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1404">
+        <v>90</v>
+      </c>
+      <c r="D1404">
+        <v>100</v>
+      </c>
+      <c r="E1404">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1405" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1405">
+        <v>90</v>
+      </c>
+      <c r="D1405">
+        <v>60</v>
+      </c>
+      <c r="E1405">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1406" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1406">
+        <v>80</v>
+      </c>
+      <c r="D1406">
+        <v>80</v>
+      </c>
+      <c r="E1406">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1407" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1407">
+        <v>100</v>
+      </c>
+      <c r="D1407">
+        <v>60</v>
+      </c>
+      <c r="E1407">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1408" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1408">
+        <v>100</v>
+      </c>
+      <c r="D1408">
+        <v>80</v>
+      </c>
+      <c r="E1408">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1409" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1409">
+        <v>100</v>
+      </c>
+      <c r="D1409">
+        <v>80</v>
+      </c>
+      <c r="E1409">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1410" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1410">
+        <v>70</v>
+      </c>
+      <c r="D1410">
+        <v>100</v>
+      </c>
+      <c r="E1410">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1411" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1411">
+        <v>40</v>
+      </c>
+      <c r="D1411">
+        <v>80</v>
+      </c>
+      <c r="E1411">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1412" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1412">
+        <v>90</v>
+      </c>
+      <c r="D1412">
+        <v>100</v>
+      </c>
+      <c r="E1412">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1413" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1413">
+        <v>100</v>
+      </c>
+      <c r="D1413">
+        <v>100</v>
+      </c>
+      <c r="E1413">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1414" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1414">
+        <v>40</v>
+      </c>
+      <c r="D1414">
+        <v>40</v>
+      </c>
+      <c r="E1414">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1415" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1415">
+        <v>100</v>
+      </c>
+      <c r="D1415">
+        <v>60</v>
+      </c>
+      <c r="E1415">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1416" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1416">
+        <v>90</v>
+      </c>
+      <c r="D1416">
+        <v>80</v>
+      </c>
+      <c r="E1416">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1417" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1417">
+        <v>90</v>
+      </c>
+      <c r="D1417">
+        <v>80</v>
+      </c>
+      <c r="E1417">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1418" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1418">
+        <v>100</v>
+      </c>
+      <c r="D1418">
+        <v>40</v>
+      </c>
+      <c r="E1418">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1419" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1419">
+        <v>100</v>
+      </c>
+      <c r="D1419">
+        <v>80</v>
+      </c>
+      <c r="E1419">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1420" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1420">
+        <v>90</v>
+      </c>
+      <c r="D1420">
+        <v>40</v>
+      </c>
+      <c r="E1420">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1421" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1421">
+        <v>90</v>
+      </c>
+      <c r="D1421">
+        <v>60</v>
+      </c>
+      <c r="E1421">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1422" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1422">
+        <v>100</v>
+      </c>
+      <c r="D1422">
+        <v>80</v>
+      </c>
+      <c r="E1422">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1423" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1423">
+        <v>50</v>
+      </c>
+      <c r="D1423">
+        <v>40</v>
+      </c>
+      <c r="E1423">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1424" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1424">
+        <v>90</v>
+      </c>
+      <c r="D1424">
+        <v>80</v>
+      </c>
+      <c r="E1424">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1425" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1425">
+        <v>80</v>
+      </c>
+      <c r="D1425">
+        <v>100</v>
+      </c>
+      <c r="E1425">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1426" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1426">
+        <v>80</v>
+      </c>
+      <c r="D1426">
+        <v>80</v>
+      </c>
+      <c r="E1426">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1427" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1427">
+        <v>90</v>
+      </c>
+      <c r="D1427">
+        <v>80</v>
+      </c>
+      <c r="E1427">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1428" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1428">
+        <v>90</v>
+      </c>
+      <c r="D1428">
+        <v>60</v>
+      </c>
+      <c r="E1428">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1429" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1429">
+        <v>90</v>
+      </c>
+      <c r="D1429">
+        <v>100</v>
+      </c>
+      <c r="E1429">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1430" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1430">
+        <v>80</v>
+      </c>
+      <c r="D1430">
+        <v>80</v>
+      </c>
+      <c r="E1430">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1431" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1431">
+        <v>90</v>
+      </c>
+      <c r="D1431">
+        <v>80</v>
+      </c>
+      <c r="E1431">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1432" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1432">
+        <v>90</v>
+      </c>
+      <c r="D1432">
+        <v>40</v>
+      </c>
+      <c r="E1432">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1433" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1433">
+        <v>80</v>
+      </c>
+      <c r="D1433">
+        <v>80</v>
+      </c>
+      <c r="E1433">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1434" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1434">
+        <v>90</v>
+      </c>
+      <c r="D1434">
+        <v>60</v>
+      </c>
+      <c r="E1434">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1435" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1435">
+        <v>70</v>
+      </c>
+      <c r="D1435">
+        <v>60</v>
+      </c>
+      <c r="E1435">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1436" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1436">
+        <v>60</v>
+      </c>
+      <c r="D1436">
+        <v>100</v>
+      </c>
+      <c r="E1436">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1437" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1437">
+        <v>30</v>
+      </c>
+      <c r="D1437">
+        <v>40</v>
+      </c>
+      <c r="E1437">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1438" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1438">
+        <v>100</v>
+      </c>
+      <c r="D1438">
+        <v>80</v>
+      </c>
+      <c r="E1438">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1439" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1439">
+        <v>50</v>
+      </c>
+      <c r="D1439">
+        <v>80</v>
+      </c>
+      <c r="E1439">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1440" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1440">
+        <v>100</v>
+      </c>
+      <c r="D1440">
+        <v>100</v>
+      </c>
+      <c r="E1440">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1441" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1441">
+        <v>90</v>
+      </c>
+      <c r="D1441">
+        <v>80</v>
+      </c>
+      <c r="E1441">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1442" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1442">
+        <v>30</v>
+      </c>
+      <c r="D1442">
+        <v>80</v>
+      </c>
+      <c r="E1442">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1443" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1443">
+        <v>50</v>
+      </c>
+      <c r="D1443">
+        <v>60</v>
+      </c>
+      <c r="E1443">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1444" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1444">
+        <v>80</v>
+      </c>
+      <c r="D1444">
+        <v>80</v>
+      </c>
+      <c r="E1444">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1445" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1445">
+        <v>60</v>
+      </c>
+      <c r="D1445">
+        <v>40</v>
+      </c>
+      <c r="E1445">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1446" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1446">
+        <v>50</v>
+      </c>
+      <c r="D1446">
+        <v>80</v>
+      </c>
+      <c r="E1446">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1447" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1447">
+        <v>100</v>
+      </c>
+      <c r="D1447">
+        <v>100</v>
+      </c>
+      <c r="E1447">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1448" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1448">
+        <v>90</v>
+      </c>
+      <c r="D1448">
+        <v>100</v>
+      </c>
+      <c r="E1448">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1449" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1449">
+        <v>80</v>
+      </c>
+      <c r="D1449">
+        <v>60</v>
+      </c>
+      <c r="E1449">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1450" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1450">
+        <v>90</v>
+      </c>
+      <c r="D1450">
+        <v>60</v>
+      </c>
+      <c r="E1450">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1451" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1451">
+        <v>60</v>
+      </c>
+      <c r="D1451">
+        <v>100</v>
+      </c>
+      <c r="E1451">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1452" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1452">
+        <v>100</v>
+      </c>
+      <c r="D1452">
+        <v>80</v>
+      </c>
+      <c r="E1452">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1453" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1453">
+        <v>70</v>
+      </c>
+      <c r="D1453">
+        <v>100</v>
+      </c>
+      <c r="E1453">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1454" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1454">
+        <v>40</v>
+      </c>
+      <c r="D1454">
+        <v>40</v>
+      </c>
+      <c r="E1454">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1455" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1455">
+        <v>90</v>
+      </c>
+      <c r="D1455">
+        <v>60</v>
+      </c>
+      <c r="E1455">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1456" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1456">
+        <v>90</v>
+      </c>
+      <c r="D1456">
+        <v>80</v>
+      </c>
+      <c r="E1456">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1457" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1457">
+        <v>90</v>
+      </c>
+      <c r="D1457">
+        <v>100</v>
+      </c>
+      <c r="E1457">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1458" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1458">
+        <v>70</v>
+      </c>
+      <c r="D1458">
+        <v>100</v>
+      </c>
+      <c r="E1458">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1459" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1459">
+        <v>60</v>
+      </c>
+      <c r="D1459">
+        <v>40</v>
+      </c>
+      <c r="E1459">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1460" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1460">
+        <v>80</v>
+      </c>
+      <c r="D1460">
+        <v>100</v>
+      </c>
+      <c r="E1460">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1461" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1461">
+        <v>70</v>
+      </c>
+      <c r="D1461">
+        <v>100</v>
+      </c>
+      <c r="E1461">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1462" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1462">
+        <v>100</v>
+      </c>
+      <c r="D1462">
+        <v>60</v>
+      </c>
+      <c r="E1462">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1463" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1463">
+        <v>90</v>
+      </c>
+      <c r="D1463">
+        <v>80</v>
+      </c>
+      <c r="E1463">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1464" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1464">
+        <v>100</v>
+      </c>
+      <c r="D1464">
+        <v>80</v>
+      </c>
+      <c r="E1464">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1465" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1465">
+        <v>70</v>
+      </c>
+      <c r="D1465">
+        <v>80</v>
+      </c>
+      <c r="E1465">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1466" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1466">
+        <v>90</v>
+      </c>
+      <c r="D1466">
+        <v>80</v>
+      </c>
+      <c r="E1466">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1467" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1467">
+        <v>100</v>
+      </c>
+      <c r="D1467">
+        <v>100</v>
+      </c>
+      <c r="E1467">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1468" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1468">
+        <v>70</v>
+      </c>
+      <c r="D1468">
+        <v>100</v>
+      </c>
+      <c r="E1468">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1469" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1469">
+        <v>70</v>
+      </c>
+      <c r="D1469">
+        <v>60</v>
+      </c>
+      <c r="E1469">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1470" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1470">
+        <v>100</v>
+      </c>
+      <c r="D1470">
+        <v>100</v>
+      </c>
+      <c r="E1470">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1471" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1471">
+        <v>90</v>
+      </c>
+      <c r="D1471">
+        <v>60</v>
+      </c>
+      <c r="E1471">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1472" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1472">
+        <v>70</v>
+      </c>
+      <c r="D1472">
+        <v>60</v>
+      </c>
+      <c r="E1472">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1473" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1473">
+        <v>90</v>
+      </c>
+      <c r="D1473">
+        <v>60</v>
+      </c>
+      <c r="E1473">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1474" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1474">
+        <v>90</v>
+      </c>
+      <c r="D1474">
+        <v>80</v>
+      </c>
+      <c r="E1474">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1475" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1475">
+        <v>70</v>
+      </c>
+      <c r="D1475">
+        <v>60</v>
+      </c>
+      <c r="E1475">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1476" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1476">
+        <v>80</v>
+      </c>
+      <c r="D1476">
+        <v>40</v>
+      </c>
+      <c r="E1476">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1477" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1477">
+        <v>80</v>
+      </c>
+      <c r="D1477">
+        <v>40</v>
+      </c>
+      <c r="E1477">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1478" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1478">
+        <v>100</v>
+      </c>
+      <c r="D1478">
+        <v>60</v>
+      </c>
+      <c r="E1478">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1479" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1479">
+        <v>90</v>
+      </c>
+      <c r="D1479">
+        <v>80</v>
+      </c>
+      <c r="E1479">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1480" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1480">
+        <v>100</v>
+      </c>
+      <c r="D1480">
+        <v>80</v>
+      </c>
+      <c r="E1480">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1481" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1481">
+        <v>100</v>
+      </c>
+      <c r="D1481">
+        <v>100</v>
+      </c>
+      <c r="E1481">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1482" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1482">
+        <v>90</v>
+      </c>
+      <c r="D1482">
+        <v>100</v>
+      </c>
+      <c r="E1482">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1483" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1483">
+        <v>100</v>
+      </c>
+      <c r="D1483">
+        <v>100</v>
+      </c>
+      <c r="E1483">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1484" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1484">
+        <v>80</v>
+      </c>
+      <c r="D1484">
+        <v>60</v>
+      </c>
+      <c r="E1484">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1485" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1485">
+        <v>80</v>
+      </c>
+      <c r="D1485">
+        <v>60</v>
+      </c>
+      <c r="E1485">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1486" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1486">
+        <v>80</v>
+      </c>
+      <c r="D1486">
+        <v>100</v>
+      </c>
+      <c r="E1486">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1487" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1487">
+        <v>100</v>
+      </c>
+      <c r="D1487">
+        <v>100</v>
+      </c>
+      <c r="E1487">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1488" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1488">
+        <v>100</v>
+      </c>
+      <c r="D1488">
+        <v>100</v>
+      </c>
+      <c r="E1488">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1489" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1489">
+        <v>80</v>
+      </c>
+      <c r="D1489">
+        <v>100</v>
+      </c>
+      <c r="E1489">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1490" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1490">
+        <v>90</v>
+      </c>
+      <c r="D1490">
+        <v>80</v>
+      </c>
+      <c r="E1490">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1491" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1491">
+        <v>100</v>
+      </c>
+      <c r="D1491">
+        <v>100</v>
+      </c>
+      <c r="E1491">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1492" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1492">
+        <v>30</v>
+      </c>
+      <c r="D1492">
+        <v>80</v>
+      </c>
+      <c r="E1492">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1493" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1493">
+        <v>70</v>
+      </c>
+      <c r="D1493">
+        <v>60</v>
+      </c>
+      <c r="E1493">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1494" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1494">
+        <v>20</v>
+      </c>
+      <c r="D1494">
+        <v>60</v>
+      </c>
+      <c r="E1494">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1495" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1495">
+        <v>80</v>
+      </c>
+      <c r="D1495">
+        <v>100</v>
+      </c>
+      <c r="E1495">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1496" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1496">
+        <v>100</v>
+      </c>
+      <c r="D1496">
+        <v>100</v>
+      </c>
+      <c r="E1496">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1497" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1497">
+        <v>50</v>
+      </c>
+      <c r="D1497">
+        <v>40</v>
+      </c>
+      <c r="E1497">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1498" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1498">
+        <v>90</v>
+      </c>
+      <c r="D1498">
+        <v>60</v>
+      </c>
+      <c r="E1498">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1499" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1499">
+        <v>100</v>
+      </c>
+      <c r="D1499">
+        <v>80</v>
+      </c>
+      <c r="E1499">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1500" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1500">
+        <v>100</v>
+      </c>
+      <c r="D1500">
+        <v>100</v>
+      </c>
+      <c r="E1500">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1501" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1501">
+        <v>90</v>
+      </c>
+      <c r="D1501">
+        <v>80</v>
+      </c>
+      <c r="E1501">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1502" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1502">
+        <v>90</v>
+      </c>
+      <c r="D1502">
+        <v>60</v>
+      </c>
+      <c r="E1502">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1503" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1503">
+        <v>100</v>
+      </c>
+      <c r="D1503">
+        <v>60</v>
+      </c>
+      <c r="E1503">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1504" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1504">
+        <v>100</v>
+      </c>
+      <c r="D1504">
+        <v>100</v>
+      </c>
+      <c r="E1504">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1505" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1505">
+        <v>90</v>
+      </c>
+      <c r="D1505">
+        <v>100</v>
+      </c>
+      <c r="E1505">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1506" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1506">
+        <v>60</v>
+      </c>
+      <c r="D1506">
+        <v>80</v>
+      </c>
+      <c r="E1506">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1507" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1507">
+        <v>100</v>
+      </c>
+      <c r="D1507">
+        <v>100</v>
+      </c>
+      <c r="E1507">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1508" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1508">
+        <v>100</v>
+      </c>
+      <c r="D1508">
+        <v>60</v>
+      </c>
+      <c r="E1508">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1509" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1509">
+        <v>50</v>
+      </c>
+      <c r="D1509">
+        <v>60</v>
+      </c>
+      <c r="E1509">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1510" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1510">
+        <v>80</v>
+      </c>
+      <c r="D1510">
+        <v>40</v>
+      </c>
+      <c r="E1510">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1511" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1511">
+        <v>60</v>
+      </c>
+      <c r="D1511">
+        <v>40</v>
+      </c>
+      <c r="E1511">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1512" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1512">
+        <v>90</v>
+      </c>
+      <c r="D1512">
+        <v>80</v>
+      </c>
+      <c r="E1512">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1513" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1513">
+        <v>80</v>
+      </c>
+      <c r="D1513">
+        <v>60</v>
+      </c>
+      <c r="E1513">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1514" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1514">
+        <v>100</v>
+      </c>
+      <c r="D1514">
+        <v>80</v>
+      </c>
+      <c r="E1514">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1515" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1515">
+        <v>50</v>
+      </c>
+      <c r="D1515">
+        <v>80</v>
+      </c>
+      <c r="E1515">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1516" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1516">
+        <v>60</v>
+      </c>
+      <c r="D1516">
+        <v>60</v>
+      </c>
+      <c r="E1516">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1517" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1517">
+        <v>90</v>
+      </c>
+      <c r="D1517">
+        <v>80</v>
+      </c>
+      <c r="E1517">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1518" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1518">
+        <v>70</v>
+      </c>
+      <c r="D1518">
+        <v>100</v>
+      </c>
+      <c r="E1518">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1519" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1519">
+        <v>0</v>
+      </c>
+      <c r="D1519">
+        <v>40</v>
+      </c>
+      <c r="E1519">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1520" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1520">
+        <v>0</v>
+      </c>
+      <c r="D1520">
+        <v>60</v>
+      </c>
+      <c r="E1520">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1521" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1521">
+        <v>80</v>
+      </c>
+      <c r="D1521">
+        <v>80</v>
+      </c>
+      <c r="E1521">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1522" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1522">
+        <v>90</v>
+      </c>
+      <c r="D1522">
+        <v>60</v>
+      </c>
+      <c r="E1522">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1523" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1523">
+        <v>40</v>
+      </c>
+      <c r="D1523">
+        <v>20</v>
+      </c>
+      <c r="E1523">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1524" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1524">
+        <v>100</v>
+      </c>
+      <c r="D1524">
+        <v>40</v>
+      </c>
+      <c r="E1524">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1525" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1525">
+        <v>80</v>
+      </c>
+      <c r="D1525">
+        <v>100</v>
+      </c>
+      <c r="E1525">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1526" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1526">
+        <v>90</v>
+      </c>
+      <c r="D1526">
+        <v>80</v>
+      </c>
+      <c r="E1526">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1527" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1527">
+        <v>60</v>
+      </c>
+      <c r="D1527">
+        <v>80</v>
+      </c>
+      <c r="E1527">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1528" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1528">
+        <v>50</v>
+      </c>
+      <c r="D1528">
+        <v>100</v>
+      </c>
+      <c r="E1528">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1529" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1529">
+        <v>90</v>
+      </c>
+      <c r="D1529">
+        <v>80</v>
+      </c>
+      <c r="E1529">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1530" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1530">
+        <v>100</v>
+      </c>
+      <c r="D1530">
+        <v>100</v>
+      </c>
+      <c r="E1530">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1531" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1531">
+        <v>80</v>
+      </c>
+      <c r="D1531">
+        <v>60</v>
+      </c>
+      <c r="E1531">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1532" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1532">
+        <v>50</v>
+      </c>
+      <c r="D1532">
+        <v>60</v>
+      </c>
+      <c r="E1532">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1533" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1533">
+        <v>100</v>
+      </c>
+      <c r="D1533">
+        <v>80</v>
+      </c>
+      <c r="E1533">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1534" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1534">
+        <v>80</v>
+      </c>
+      <c r="D1534">
+        <v>100</v>
+      </c>
+      <c r="E1534">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1535" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1535">
+        <v>100</v>
+      </c>
+      <c r="D1535">
+        <v>100</v>
+      </c>
+      <c r="E1535">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1536" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1536">
+        <v>100</v>
+      </c>
+      <c r="D1536">
+        <v>80</v>
+      </c>
+      <c r="E1536">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1537" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1537">
+        <v>90</v>
+      </c>
+      <c r="D1537">
+        <v>80</v>
+      </c>
+      <c r="E1537">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1538" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1538">
+        <v>100</v>
+      </c>
+      <c r="D1538">
+        <v>100</v>
+      </c>
+      <c r="E1538">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1539" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1539">
+        <v>60</v>
+      </c>
+      <c r="D1539">
+        <v>80</v>
+      </c>
+      <c r="E1539">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1540" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1540">
+        <v>80</v>
+      </c>
+      <c r="D1540">
+        <v>60</v>
+      </c>
+      <c r="E1540">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1541" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1541">
+        <v>100</v>
+      </c>
+      <c r="D1541">
+        <v>80</v>
+      </c>
+      <c r="E1541">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1542" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1542">
+        <v>90</v>
+      </c>
+      <c r="D1542">
+        <v>40</v>
+      </c>
+      <c r="E1542">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1543" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1543">
+        <v>100</v>
+      </c>
+      <c r="D1543">
+        <v>100</v>
+      </c>
+      <c r="E1543">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1544" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1544">
+        <v>90</v>
+      </c>
+      <c r="D1544">
+        <v>80</v>
+      </c>
+      <c r="E1544">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1545" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1545">
+        <v>100</v>
+      </c>
+      <c r="D1545">
+        <v>100</v>
+      </c>
+      <c r="E1545">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1546" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1546">
+        <v>100</v>
+      </c>
+      <c r="D1546">
+        <v>40</v>
+      </c>
+      <c r="E1546">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1547" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1547">
+        <v>0</v>
+      </c>
+      <c r="D1547">
+        <v>60</v>
+      </c>
+      <c r="E1547">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1548" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1548">
+        <v>60</v>
+      </c>
+      <c r="D1548">
+        <v>80</v>
+      </c>
+      <c r="E1548">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1549" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1549">
+        <v>50</v>
+      </c>
+      <c r="D1549">
+        <v>100</v>
+      </c>
+      <c r="E1549">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1550" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1550">
+        <v>100</v>
+      </c>
+      <c r="D1550">
+        <v>100</v>
+      </c>
+      <c r="E1550">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1551" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1551">
+        <v>60</v>
+      </c>
+      <c r="D1551">
+        <v>80</v>
+      </c>
+      <c r="E1551">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1552" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1552">
+        <v>100</v>
+      </c>
+      <c r="D1552">
+        <v>80</v>
+      </c>
+      <c r="E1552">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1553" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1553">
+        <v>60</v>
+      </c>
+      <c r="D1553">
+        <v>60</v>
+      </c>
+      <c r="E1553">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1554" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1554">
+        <v>100</v>
+      </c>
+      <c r="D1554">
+        <v>100</v>
+      </c>
+      <c r="E1554">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1555" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1555">
+        <v>70</v>
+      </c>
+      <c r="D1555">
+        <v>100</v>
+      </c>
+      <c r="E1555">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1556" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1556">
+        <v>100</v>
+      </c>
+      <c r="D1556">
+        <v>100</v>
+      </c>
+      <c r="E1556">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1557" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1557">
+        <v>80</v>
+      </c>
+      <c r="D1557">
+        <v>80</v>
+      </c>
+      <c r="E1557">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1558" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1558">
+        <v>60</v>
+      </c>
+      <c r="D1558">
+        <v>40</v>
+      </c>
+      <c r="E1558">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1559" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1559">
+        <v>100</v>
+      </c>
+      <c r="D1559">
+        <v>60</v>
+      </c>
+      <c r="E1559">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1560" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1560">
+        <v>90</v>
+      </c>
+      <c r="D1560">
+        <v>80</v>
+      </c>
+      <c r="E1560">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1561" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1561">
+        <v>90</v>
+      </c>
+      <c r="D1561">
+        <v>100</v>
+      </c>
+      <c r="E1561">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1562" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1562">
+        <v>100</v>
+      </c>
+      <c r="D1562">
+        <v>60</v>
+      </c>
+      <c r="E1562">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1563" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1563">
+        <v>100</v>
+      </c>
+      <c r="D1563">
+        <v>100</v>
+      </c>
+      <c r="E1563">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1564" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1564">
+        <v>80</v>
+      </c>
+      <c r="D1564">
+        <v>80</v>
+      </c>
+      <c r="E1564">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1565" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1565">
+        <v>60</v>
+      </c>
+      <c r="D1565">
+        <v>60</v>
+      </c>
+      <c r="E1565">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1566" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1566">
+        <v>90</v>
+      </c>
+      <c r="D1566">
+        <v>40</v>
+      </c>
+      <c r="E1566">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1567" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1567">
+        <v>40</v>
+      </c>
+      <c r="D1567">
+        <v>40</v>
+      </c>
+      <c r="E1567">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1568" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1568">
+        <v>100</v>
+      </c>
+      <c r="D1568">
+        <v>100</v>
+      </c>
+      <c r="E1568">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1569" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1569">
+        <v>80</v>
+      </c>
+      <c r="D1569">
+        <v>80</v>
+      </c>
+      <c r="E1569">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1570" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1570">
+        <v>80</v>
+      </c>
+      <c r="D1570">
+        <v>100</v>
+      </c>
+      <c r="E1570">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1571" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1571">
+        <v>100</v>
+      </c>
+      <c r="D1571">
+        <v>20</v>
+      </c>
+      <c r="E1571">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1572" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1572">
+        <v>100</v>
+      </c>
+      <c r="D1572">
+        <v>60</v>
+      </c>
+      <c r="E1572">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1573" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1573">
+        <v>100</v>
+      </c>
+      <c r="D1573">
+        <v>100</v>
+      </c>
+      <c r="E1573">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1574" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1574">
+        <v>70</v>
+      </c>
+      <c r="D1574">
+        <v>80</v>
+      </c>
+      <c r="E1574">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1575" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1575">
+        <v>30</v>
+      </c>
+      <c r="D1575">
+        <v>80</v>
+      </c>
+      <c r="E1575">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1576" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1576">
+        <v>80</v>
+      </c>
+      <c r="D1576">
+        <v>80</v>
+      </c>
+      <c r="E1576">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1577" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1577">
+        <v>90</v>
+      </c>
+      <c r="D1577">
+        <v>60</v>
+      </c>
+      <c r="E1577">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1578" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1578">
+        <v>50</v>
+      </c>
+      <c r="D1578">
+        <v>80</v>
+      </c>
+      <c r="E1578">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1579" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1579">
+        <v>10</v>
+      </c>
+      <c r="D1579">
+        <v>80</v>
+      </c>
+      <c r="E1579">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1580" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1580">
+        <v>80</v>
+      </c>
+      <c r="D1580">
+        <v>80</v>
+      </c>
+      <c r="E1580">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1581" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1581">
+        <v>80</v>
+      </c>
+      <c r="D1581">
+        <v>100</v>
+      </c>
+      <c r="E1581">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1582" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1582">
+        <v>40</v>
+      </c>
+      <c r="D1582">
+        <v>60</v>
+      </c>
+      <c r="E1582">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1583" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1583">
+        <v>10</v>
+      </c>
+      <c r="D1583">
+        <v>40</v>
+      </c>
+      <c r="E1583">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1584" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1584">
+        <v>30</v>
+      </c>
+      <c r="D1584">
+        <v>60</v>
+      </c>
+      <c r="E1584">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1585" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1585">
+        <v>90</v>
+      </c>
+      <c r="D1585">
+        <v>100</v>
+      </c>
+      <c r="E1585">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1586" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1586">
+        <v>30</v>
+      </c>
+      <c r="D1586">
+        <v>100</v>
+      </c>
+      <c r="E1586">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1587" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1587">
+        <v>30</v>
+      </c>
+      <c r="D1587">
+        <v>100</v>
+      </c>
+      <c r="E1587">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1588" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1588">
+        <v>60</v>
+      </c>
+      <c r="D1588">
+        <v>80</v>
+      </c>
+      <c r="E1588">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1589" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1589">
+        <v>90</v>
+      </c>
+      <c r="D1589">
+        <v>80</v>
+      </c>
+      <c r="E1589">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1590" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1590">
+        <v>50</v>
+      </c>
+      <c r="D1590">
+        <v>80</v>
+      </c>
+      <c r="E1590">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1591" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1591">
+        <v>60</v>
+      </c>
+      <c r="D1591">
+        <v>40</v>
+      </c>
+      <c r="E1591">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1592" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1592">
+        <v>60</v>
+      </c>
+      <c r="D1592">
+        <v>80</v>
+      </c>
+      <c r="E1592">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1593" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1593">
+        <v>30</v>
+      </c>
+      <c r="D1593">
+        <v>40</v>
+      </c>
+      <c r="E1593">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1594" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1594">
+        <v>40</v>
+      </c>
+      <c r="D1594">
+        <v>20</v>
+      </c>
+      <c r="E1594">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1595" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1595">
+        <v>0</v>
+      </c>
+      <c r="D1595">
+        <v>0</v>
+      </c>
+      <c r="E1595">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1596" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1596">
+        <v>70</v>
+      </c>
+      <c r="D1596">
+        <v>100</v>
+      </c>
+      <c r="E1596">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1597" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1597">
+        <v>90</v>
+      </c>
+      <c r="D1597">
+        <v>80</v>
+      </c>
+      <c r="E1597">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1598" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1598">
+        <v>80</v>
+      </c>
+      <c r="D1598">
+        <v>100</v>
+      </c>
+      <c r="E1598">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1599" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1599">
+        <v>90</v>
+      </c>
+      <c r="D1599">
+        <v>80</v>
+      </c>
+      <c r="E1599">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1600" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1600">
+        <v>60</v>
+      </c>
+      <c r="D1600">
+        <v>100</v>
+      </c>
+      <c r="E1600">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1601" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1601">
+        <v>100</v>
+      </c>
+      <c r="D1601">
+        <v>100</v>
+      </c>
+      <c r="E1601">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1602" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1602">
+        <v>60</v>
+      </c>
+      <c r="D1602">
+        <v>60</v>
+      </c>
+      <c r="E1602">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1603" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1603">
+        <v>80</v>
+      </c>
+      <c r="D1603">
+        <v>60</v>
+      </c>
+      <c r="E1603">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1604" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1604">
+        <v>90</v>
+      </c>
+      <c r="D1604">
+        <v>100</v>
+      </c>
+      <c r="E1604">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1605" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1605">
+        <v>100</v>
+      </c>
+      <c r="D1605">
+        <v>80</v>
+      </c>
+      <c r="E1605">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1606" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1606">
+        <v>0</v>
+      </c>
+      <c r="D1606">
+        <v>0</v>
+      </c>
+      <c r="E1606">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1607" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1607">
+        <v>70</v>
+      </c>
+      <c r="D1607">
+        <v>40</v>
+      </c>
+      <c r="E1607">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1608" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1608">
+        <v>60</v>
+      </c>
+      <c r="D1608">
+        <v>40</v>
+      </c>
+      <c r="E1608">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1609" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1609">
+        <v>100</v>
+      </c>
+      <c r="D1609">
+        <v>80</v>
+      </c>
+      <c r="E1609">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1610" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1610">
+        <v>70</v>
+      </c>
+      <c r="D1610">
+        <v>40</v>
+      </c>
+      <c r="E1610">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1611" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1611">
+        <v>20</v>
+      </c>
+      <c r="D1611">
+        <v>60</v>
+      </c>
+      <c r="E1611">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1612" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1612">
+        <v>40</v>
+      </c>
+      <c r="D1612">
+        <v>80</v>
+      </c>
+      <c r="E1612">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1613" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1613">
+        <v>90</v>
+      </c>
+      <c r="D1613">
+        <v>60</v>
+      </c>
+      <c r="E1613">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1614" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1614">
+        <v>80</v>
+      </c>
+      <c r="D1614">
+        <v>100</v>
+      </c>
+      <c r="E1614">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1615" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1615">
+        <v>80</v>
+      </c>
+      <c r="E1615">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>